<commit_message>
Atualização - Base + textos
</commit_message>
<xml_diff>
--- a/assets/Loki_aleatório.xlsx
+++ b/assets/Loki_aleatório.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Matérias 2 semestre\cdados\P1\Classificador_automatico_de_sentimentos\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEC03DF-3403-477E-96EA-1C2268ADE027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D703C99-8B73-496B-ADA0-975B5DB63A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B784BBDE-8CAE-4A9A-97CC-F00DF2CF51F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B784BBDE-8CAE-4A9A-97CC-F00DF2CF51F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="1002">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2676,12 +2676,680 @@
   <si>
     <t>Teste</t>
   </si>
+  <si>
+    <t>@loki_trem @pain_krzn @cacauzinha_ff @fluxo_alemaze tava pensando em outra pessoa mas neee</t>
+  </si>
+  <si>
+    <t>@pombodopru @peterjordan100 se a avt fica fora dos multiversos e do tempo, pq ao final de loki os caras ñ lembram dele ?</t>
+  </si>
+  <si>
+    <t>@loki_cb mas nesse desenho eu não curti, ent apaguei-</t>
+  </si>
+  <si>
+    <t>no final de deadpool 2 ele volta no tempo e muda tudo, e se isso fizesse com que deadpool fosse capturado pela tva 👀👀👀
+#deadpool #loki  #crossover</t>
+  </si>
+  <si>
+    <t>@seokjincomics a surra no tony, natasha e loki que tão mortos https://t.co/n3fhdjc55e</t>
+  </si>
+  <si>
+    <t>quinta e sexta: wandavision 
+sábado: the falcon and the winter soldier 
+domingo: loki 
+programação de covid com ed</t>
+  </si>
+  <si>
+    <t>@hcneyhyvck obrigada flor</t>
+  </si>
+  <si>
+    <t>adorei o primeiro epi de loki, será que a marvel entregou outra série boa depois do fracasso de tfatws</t>
+  </si>
+  <si>
+    <t>eu tive uma interação muito estranha com o loki quando eu tava deitada
+👩🏻‍🦰...
+😼...
+👩🏻‍🦰...
+😼...
+👩🏻‍🦰...
+😼...
+👩🏻‍🦰...
+😼 *morde minha barriga do nada*</t>
+  </si>
+  <si>
+    <t>tem alg no portao falando c loki q odio</t>
+  </si>
+  <si>
+    <t>• homem de ferro
+• loki: agente de asgard https://t.co/clxhn4u1it</t>
+  </si>
+  <si>
+    <t>@lllrieieiei @rsrssep mesmo assim era pra ter mais</t>
+  </si>
+  <si>
+    <t>vou assistir loki de novo</t>
+  </si>
+  <si>
+    <t>mds eu tô block de três dias</t>
+  </si>
+  <si>
+    <t>esqueceu do loki do eixo bebê novo herói kkkkkkkkkkk https://t.co/bjm6gtvcb8</t>
+  </si>
+  <si>
+    <t>@saturnmagno no tópico do loki só tem au, pov e fanart de sylkie eu fico exatamente assim https://t.co/z4acl9ipmy</t>
+  </si>
+  <si>
+    <t>@yoonpoemz mas sou eu taty?</t>
+  </si>
+  <si>
+    <t>@loki_bra se enviarem o primeiro ep o tom hiddleston talvez seja indicado.</t>
+  </si>
+  <si>
+    <t>@jojogum13 com certeza chiclete daqueles q todo  mundo gosta.</t>
+  </si>
+  <si>
+    <t>borel completamente doente, tem que chegar nas ideia com um loki desse!</t>
+  </si>
+  <si>
+    <t>lista dos 300 motivos mostrando que loki e sylvie não são irmãos... https://t.co/9twmiq89zn</t>
+  </si>
+  <si>
+    <t>caralho loki para de latir</t>
+  </si>
+  <si>
+    <t>16- ele faz o justo! tyr o deus nórdico, tem algumas semelhanças com o “ruivo.”
+no conto nórdico, quando os deuses perceberam que, segundo o oráculo, os filhos de loki ameaçavam fazer desgraças pela terra, decidiram então prender o lobo fenris. https://t.co/geitkkfxko</t>
+  </si>
+  <si>
+    <t>@melhornao777 @loki_trem @bakzinfx7 @loud_thurzin888 @bakzera aliás, quer uma??</t>
+  </si>
+  <si>
+    <t>@joanabizarro o loki é obediente... se achar que eu não o apanho é um anjo. 😇
+já se pensar que tão cedo não lhe ponho as mãos em cima...
+o que mais adoro nele é que, mesmo após estes anos todos, em nada se acha inferior a mim, e se faz o que lhe digo é pq não está para me aturar 🙃</t>
+  </si>
+  <si>
+    <t>@scarletscoeur loki e tony no comando da sua personalidade kkkkkk,deveria de preocupar amg??</t>
+  </si>
+  <si>
+    <t>@melhornao777 @loki_trem @bakzinfx7 @loud_thurzin888 @bakzera só isso msm, pq nfa pipocou, camp do próprio dono da org pipocou nos dois e os outros tbm kkkkkkk</t>
+  </si>
+  <si>
+    <t>@carpntevol sim
+jenny agora que eu tô vendo loki tenho certeza que que ele vai achar um jeito de continuar vivo</t>
+  </si>
+  <si>
+    <t>@loki_trem @pain_krzn @cacauzinha_ff @fluxo_alemaze já falaram q foi ela?</t>
+  </si>
+  <si>
+    <t>desejado por jogadores avançados, loki oferece uma variedade de habilidades especializadas de reconfiguração. a criatividade dos poderes de loki permite aos jogadores dominar o campo de batalha por meio da manipulação.</t>
+  </si>
+  <si>
+    <t>@kkkkkkkkk0i00 @samuelmenor14 @rafaelfmsilva @peterjordan100 loki acontece antes de endgame (2012), mas o templo do kang e a avt são atemporais</t>
+  </si>
+  <si>
+    <t>te amo loki, eu te amo...</t>
+  </si>
+  <si>
+    <t>gente eu tinha uma teoria muito doid de que o kian quando "matava" as pessoas era igual em loki q elas so iriam oara outro mundo</t>
+  </si>
+  <si>
+    <t>@huwtaos achei q tava falando de loki,,
+fiquei "elysia???"</t>
+  </si>
+  <si>
+    <t>@hiddlesloversbz eu nao shippo loki e a sylvie mas adm vc esta certissime 
+e quem nao ve é pq num quer viu</t>
+  </si>
+  <si>
+    <t>@hanherond o loki eh maluco igual eu vai dar td certo</t>
+  </si>
+  <si>
+    <t>@7delo confia</t>
+  </si>
+  <si>
+    <t>@lalaxzyy pode sim mo</t>
+  </si>
+  <si>
+    <t>@sazo0n mttttt..... eh esses loki q vão lotar hospital dnv doente dessa merda</t>
+  </si>
+  <si>
+    <t>@winixcrf tiu novi traidor</t>
+  </si>
+  <si>
+    <t>@loki_inluv entendo meu bem, melhoras 😢</t>
+  </si>
+  <si>
+    <t>o gráfico de loki eh a coisa mais linda do mundo serio o começo do último ep mostrando o universo foi espetacular q coisa lindaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>@laysatribbiani sei só primo skskks, mas se o loki é teu brother o thor tbm skskskks</t>
+  </si>
+  <si>
+    <t>@nothermoreira sim, e eu espero que aposentem ele mesmo... clint é um dos meus personagens favoritos, mas esse do mcu não dá não.
+simm, espero que seja boa. apesar que nem loki eu vi ainda 👀</t>
+  </si>
+  <si>
+    <t>@ikuyuyuki juro, loki é esperto, tal qual o nome</t>
+  </si>
+  <si>
+    <t>@hanherond gente q lerdrza essa minha enfim
+o dobby é lindo mesmo puxou a mamãe, ele e o loki serão best friends igual nos duas</t>
+  </si>
+  <si>
+    <t>@xnymeria_ ma povero loki 🥺</t>
+  </si>
+  <si>
+    <t>eles me mamam tanto, que o nome do grupo é loki pai de todos nós. https://t.co/pnfxz96zgi</t>
+  </si>
+  <si>
+    <t>e q ele não tava no controle de tudo, e era exatamente isso q o tom queria, ele queria algo novo p poder fazer uma redenção boa pro loki e colocar ele numa posição onde ele aprendesse a ser mais humilde, infelizmente esse pessoal odiou a série por isso e eu só lamento pq eu amei</t>
+  </si>
+  <si>
+    <t>minha cunhada faz amigurumi, ela fez o capitão américa. é muito abuso eu pedir pra ela fazer um loki pra mim ? 🥺🙄 
+ela não faz pra vender. 😬</t>
+  </si>
+  <si>
+    <t>@sylvielaufeydit @bracinhodeferro @meupai_eadory pq vc e o loki são tão frios ?</t>
+  </si>
+  <si>
+    <t>@prisciiart a segunda temporada vai ter um foco do loki procurando pela sylvie, então acho que vamos ver muito do relacionamento deles e o desenvolvimento aos poucos. na s1, realmente, eles não entendiam os sentimentos, então dá um de ar "hum, não vai dar certo... hum, meio estranho"</t>
+  </si>
+  <si>
+    <t>a essa altura do campeonato, quando eu vejo gente falando que loki foi ruim eu só fico 🥺🥺🥺</t>
+  </si>
+  <si>
+    <t>@oocrafa_ @melhornao777 @robertpdm @cebolafalpadol @cri4s_rs @bakzera @el_ruan77 mobile é uma desgraça kkk errando as letra</t>
+  </si>
+  <si>
+    <t>tony e loki com as maiores porcentagens uepa https://t.co/hz46210vh9</t>
+  </si>
+  <si>
+    <t>@m1kefrog vai lá loki</t>
+  </si>
+  <si>
+    <t>karaio terminei loki, só consigo pensar, quando vai aparecer minha variante para eu viver um romance comigo mesmo ???</t>
+  </si>
+  <si>
+    <t>faça o cosplay de loki logo isso é uma ameaça 🗡️ @stormwookiee https://t.co/k9qa7iwpcp</t>
+  </si>
+  <si>
+    <t>@howardst4rk jane solo jugaba, loki estaba histérico por ganar kskskakak</t>
+  </si>
+  <si>
+    <t>@rsrssep kkk ff ta flopado</t>
+  </si>
+  <si>
+    <t>@hiddlesylki era o loki e a sylvie do seu edit 
+fonte: nao preciso https://t.co/srbho1ycyh</t>
+  </si>
+  <si>
+    <t>nao posso me matsr ainda pq nao saiu a segunda temporada de loki</t>
+  </si>
+  <si>
+    <t>@loloromanoff loki e stark divos https://t.co/0vyyprex7g</t>
+  </si>
+  <si>
+    <t>@20bluebutterfly @jeangrangerw eu vi isso! 😂😂😂😂 eu dei muita risada. é um tipo diferente de shipper e eu vivo por isso
+lembro do meme que uma página fez do loki perguntando aos timekeepers: se eu pegar a syl [primeira vez que vi alguém se referindo à sylvie como syl e eu amei] vai ser sex* ou mast*rbação?</t>
+  </si>
+  <si>
+    <t>eu sonhei que o loki tinha ficado puto cmg e me mandou pra outra encarnação?????? cara que sonho bizarro</t>
+  </si>
+  <si>
+    <t>@manoreiss so sabe reclamar loki vai la e faz o seu</t>
+  </si>
+  <si>
+    <t>sério não entra na minha cabeça que o loki o deus da mentira e da trapaça que já fingiu sua própria morte foi tão burro em tentar matar o thanos com uma faquinha de pão tipo ????? eu não aceito isso</t>
+  </si>
+  <si>
+    <t>@goddessguy fiquei 75% loki e hulk foram os maiores kkkk</t>
+  </si>
+  <si>
+    <t>tô loki</t>
+  </si>
+  <si>
+    <t>e ainda veio falar cmg, sinceramente 👎🏻👎🏻👎🏻👎🏻👎🏻👎🏻👎🏻👎🏻👎🏻 e minha vó invés de defender nois eh outra pilantra sem vergonha. família eh um caralho memo, p mim eh parente. família eh diferente, até quem não eh meu sangue eh mais família q esses loki</t>
+  </si>
+  <si>
+    <t>@loloromanoff loki e viúva negra https://t.co/op5obopc5v</t>
+  </si>
+  <si>
+    <t>@altaexposicao loki e evelyn hugo meus xodós 🥺💞💞</t>
+  </si>
+  <si>
+    <t>@gkplait ateu</t>
+  </si>
+  <si>
+    <t>vcs querem usar ragnarok como base pra personalidade do loki é foda viu!!</t>
+  </si>
+  <si>
+    <t>@pombodopru @samuelmenor14 @rafaelfmsilva @peterjordan100 me responde pq o loki foi preso então</t>
+  </si>
+  <si>
+    <t>@mightyjane_ no me importa, foster</t>
+  </si>
+  <si>
+    <t>o pessoal achar q eles são o mesmo loki, eu até entendo, mas irmãos? ces tao drogado? https://t.co/ovzxmlwbg9</t>
+  </si>
+  <si>
+    <t>@kkkkkkkkk0i00 @peterjordan100 end game não é uma variante porque deveria ter acontecido na linha do tempo sagrada, eles explicaram no ep 1 de loki</t>
+  </si>
+  <si>
+    <t>@dicecream2 @nhitosa1 @beastarsz @aphroditeamone1 krl olha isso</t>
+  </si>
+  <si>
+    <t>@barcombruss @bellend20201 @attorneyjeremy1 @cryztalseth é uma complementação da mensagem… jeremy tem feitos denúncias substanciais contra sec por ter funcionários se aproveitando das regulações que deixam de fazer, em benefício próprio, enquanto prejudicam quem deveriam proteger. o loki faz algo parecido, não?</t>
+  </si>
+  <si>
+    <t>gente, ainda não assisti venom, loki, what if , e as novas temporadas de la casa de papel e sex education...</t>
+  </si>
+  <si>
+    <t>@favzinha sempre deu certo viu? eu disse que se o loki continuasse vivo na série, eu ia fazer uma tatuagem dele… adivinha oq eu tenho na perna</t>
+  </si>
+  <si>
+    <t>@pcybbhk o loki fugiu???</t>
+  </si>
+  <si>
+    <t>minha mãe só chamar o loki de low key low key e eu culpo a ally</t>
+  </si>
+  <si>
+    <t>a gatinha do meu irmão é muito fofinha, uma pena que ela não foi muito com a cara do loki kkkkkk kyra é muito fofinha https://t.co/youwwcrwsd</t>
+  </si>
+  <si>
+    <t>nada me tira da cabeça que o sinal dos 10 anéis recebeu da linha do tempo, tem a ver c o homem aranha, loki e wanda!!!</t>
+  </si>
+  <si>
+    <t>@paulswartt @hiddleself então você é a alma boa que vai me emprestar a disney+ para eu assistir a série do meu marido?(loki</t>
+  </si>
+  <si>
+    <t>@lwtbraveasf nomes da marvel. aorjdi se eu fosse marvete na época q o nick era bb eu ctz teria dado nome de tony ou loki</t>
+  </si>
+  <si>
+    <t>@softhiddlexs eu sou o loki em pessoa amou? https://t.co/jhy1vn3iij</t>
+  </si>
+  <si>
+    <t>@mateuspinguim77 @pain_luca33 vc só tem seguidores por causa de ff kkkk , esse lol aí é falido</t>
+  </si>
+  <si>
+    <t>hoje ganhei da minha cunhada esse quadro lindo pintado à mão tirado de uma foto minha com os gatos aqui de casa. ela viu que eu postei que tava com saudade do loki que partiu ano passado e teve a delicadeza de incluir meu peto na imagem 🖤
+chorei igual uma vaca véia 😭 https://t.co/imomvc3j3g</t>
+  </si>
+  <si>
+    <t>descobri que a pronuncia certa de loki é lhoaki, falava o nome do meu pai errado. https://t.co/5pofuolman</t>
+  </si>
+  <si>
+    <t>loki explicando as coisas todo feliz ;(</t>
+  </si>
+  <si>
+    <t>@melhornao777 @loki_trem @bakzinfx7 @loud_thurzin888 @bakzera tá ficando putin ja?</t>
+  </si>
+  <si>
+    <t>saudade do loki</t>
+  </si>
+  <si>
+    <t>• fabulosos vingadores: os gêmeos do apocalipse 
+• o poderoso thor ragnarok
+• thor: o último viking
+• os julgamentos de loki https://t.co/jxw2ggrvkc</t>
+  </si>
+  <si>
+    <t>@artutubr seria essa mais uma variante do loki?</t>
+  </si>
+  <si>
+    <t>pensando se assistir loki vai diminuir a minha vontade de ******.</t>
+  </si>
+  <si>
+    <t>em quais categorias vocês acham que 'loki' poderia ser indicada no #emmys 2022 ??? https://t.co/befvqecbsr</t>
+  </si>
+  <si>
+    <t>@loki_inluv tudo bem??</t>
+  </si>
+  <si>
+    <t>cade o loki bonito?????? https://t.co/qtdwdhkzsp</t>
+  </si>
+  <si>
+    <t>@sashckerman na verdade ele smp foi aquilo ali, mas o pessoal endeusava um lado dele que nunca foi real, loki smp foi babão pelo irmão, amou odin mesmo depois de saber a verdade e na serie mostrou apenas como ele reagiu a tudo isso pela narrativa dele mesmo</t>
+  </si>
+  <si>
+    <t>@rsrssep @loki_trem claro, hoje só tem loud de hype, ontem tinha fluxo e los</t>
+  </si>
+  <si>
+    <t>se o loki errou foi tentando acertar e digo mais !</t>
+  </si>
+  <si>
+    <t>jinjer anuncia data extra em são paulo e shows em curitiba e porto alegre https://t.co/nqf241bjia</t>
+  </si>
+  <si>
+    <t>@digg0__ os mais loki</t>
+  </si>
+  <si>
+    <t>@kkkkkkkkk0i00 @peterjordan100 quem construiu a avt foi ele, mas se ele aparecesse lá ninguém saberia, igual o loki que tá cheio de arquivo dele como procurado na avt e ninguém sabe quem é. ele disse que um kang do mal assumiria mas não é instantaneamente, você tá pegando coisas aleatórias e criando teorias</t>
+  </si>
+  <si>
+    <t>@fandomfx @robertpdm @yurixl15 @daaygamer @cacauzinha_ff sai dai criança da fluxo</t>
+  </si>
+  <si>
+    <t>loki me acordou às 6hrs da manhã reclamando, como se estivesse querendo comer, coloquei a comida e ele não quis, o meliante queria brincar.
+a foto do meliante: https://t.co/t3cpa0sdf6</t>
+  </si>
+  <si>
+    <t>o loki realizou meu sonho sim</t>
+  </si>
+  <si>
+    <t>@moonyhaku plmns é o loki kkk https://t.co/hq1oa6bzjk</t>
+  </si>
+  <si>
+    <t>@sashckerman loki versão marvel é do bem. pra mim, loki mesmo era o do primeiro filme do thor e avengers. eu amei a série loki, mas ela é puro funservice.</t>
+  </si>
+  <si>
+    <t>@vandamepappylon muito igual o loki</t>
+  </si>
+  <si>
+    <t>@pvd_mumuu kkkk que isso loki</t>
+  </si>
+  <si>
+    <t>@larymmotta assisti o 1° ep esses dias e gostei, mas também né loki = ❤</t>
+  </si>
+  <si>
+    <t>@pain_krzn @fc_jjordan @cacauzinha_ff @fluxo_alemaze não pode é namoro sério kkk</t>
+  </si>
+  <si>
+    <t>@loki_trem @fc_jjordan @cacauzinha_ff @fluxo_alemaze ah sla, os mano aq disseram que tem um tweet ai dizendo que não pode '-' to entendendo mais nada</t>
+  </si>
+  <si>
+    <t>¿a loki o a thor? ¿o a ambos? https://t.co/robckldhsv</t>
+  </si>
+  <si>
+    <t>@loki_trem @fc_jjordan @cacauzinha_ff @fluxo_alemaze mas não tem sentido, pq não pode ter relacionamento entre os membros, eu acho '-'</t>
+  </si>
+  <si>
+    <t>terminei sex education, vou aproveitar esse domingo de ressaca pra ver loki e what if...?</t>
+  </si>
+  <si>
+    <t>@jb_ninguem @loki_trem ontem pego 130k  espera a próxima semana e vc vai ver a diferença 😬</t>
+  </si>
+  <si>
+    <t>@puddingarts te dou de presente só pelo tanto de status q postei.</t>
+  </si>
+  <si>
+    <t>tempo pelo e também um pouco dos truques de #loki. 
+era mais do que apenas uma cor, já que os anéis também se comportavam de maneira diferente com cada portador. quando #wenwu os usou, os anéis eram "muito pontiagudos e agressivos", enquanto o uso que #shangchi fez deles se [+] https://t.co/g6knmrvol9</t>
+  </si>
+  <si>
+    <t>a msrvel é tão burra que preferiu colocar a hela como irmã do loki ao invés de colocar ela como filha dele com a amora e usar boa parte da mitologia a favor disso kakakakka</t>
+  </si>
+  <si>
+    <t>@20bluebutterfly @jeangrangerw eu quero muito encontrar esse meme de novo. é só muito bom.
+eu amo que a galera acolheu o loki como "olha aí, se até o loki pode se apaixonar e 'gadar', porque e não posso?"</t>
+  </si>
+  <si>
+    <t>a um passo de maratonar loki de novo</t>
+  </si>
+  <si>
+    <t>alguem me da uma conta da disney plus quero ve loki</t>
+  </si>
+  <si>
+    <t>mds esse livro do loki é tão bom n quero acabar ele</t>
+  </si>
+  <si>
+    <t>@rsrssep @loki_trem ja bugou uma vez, quando a loud foi pra respescagem, tinha os prêmios da final, e deu mó rolo pq pra algumas pessoas bateu as metas e pra outras não</t>
+  </si>
+  <si>
+    <t>é assim que você demonstra que se importou? meus parabéns🥰☺️</t>
+  </si>
+  <si>
+    <t>@loki_cb fique a vontade meu perfil na twitch é puddingartss #paz</t>
+  </si>
+  <si>
+    <t>@wonderwordd 1 - viúva negra
+2 - wanda
+3 - loki
+4 - thor
+5 - doutor estranho</t>
+  </si>
+  <si>
+    <t>o loki todo de terno preto pisa no thor
+nunca achei que iria ter crush num emo</t>
+  </si>
+  <si>
+    <t>loki abraçando a frida :(((</t>
+  </si>
+  <si>
+    <t>todo dia o funko do loki tá numa posição diferente. uma vez ele sumiu por vários dias, quando desisti de procurar ele apareceu em outro cômodo (ninguém tinha vindo em casa).
+deveria me preocupar?</t>
+  </si>
+  <si>
+    <t>pra qm é dedicado seu fc?
+🌷icon: alex 
+🍧header: gilmore girls
+🎂user: niall
+☁️nome: apelido, símbolo do loki e stan da lauren graham
+🍙bio: lorelai 
+🍥localização: gilmore girls 
+🍡site: sam winchester 
+🍚fixado: minha loja 
+kibei</t>
+  </si>
+  <si>
+    <t>@pombodopru @samuelmenor14 @rafaelfmsilva @peterjordan100 claro q é possível ter a disponibilade do multiverso antes, só q ninguem a usou por n motivos. e se vc lembrar, no ultimato os caras tem q viajar mais no passado depois q o loki foge com o quadrado lá e em loki, o próprio é preso por ter roubado esse quadrado, ou seja, a viagem+</t>
+  </si>
+  <si>
+    <t>pensando em ver loki pela 1534273 vez</t>
+  </si>
+  <si>
+    <t>a carinha do loki quando o odin fala que a frigga teria orgulho dele e que ele o ama 🤏🏻😭😭😭</t>
+  </si>
+  <si>
+    <t>se um dia eu fui triste não lembro!!! o meu deu loki e o de vcs???? https://t.co/5vafehworr</t>
+  </si>
+  <si>
+    <t>eu fiz o cosplay de loki e fiquei tão bonita pena que não vou postar 😭</t>
+  </si>
+  <si>
+    <t>@lock_0ff @gueguelblack @_riosx loki, vc por aqui...</t>
+  </si>
+  <si>
+    <t>@vminsepega manda ele tomar no cu, da um feche nele</t>
+  </si>
+  <si>
+    <t>achei umas fotos e vídeos do loki, deu uma tristeza e saudade do meu bebê</t>
+  </si>
+  <si>
+    <t>loki nem é série, é uma obra de arte! 💚</t>
+  </si>
+  <si>
+    <t>@marohzinha__ você é a melhor! não pensa assim</t>
+  </si>
+  <si>
+    <t>praticamente obriguei a mh mãe a ver loki comigo e ela achou de bom tom praticamente me obrigar a ver lupin com ela. já dormi e acordei umas três vezes e essa série não acaba</t>
+  </si>
+  <si>
+    <t>não entendi pq não gostaram de loki, eu adorei kkk 
+não tinha como sair do buraco que inventaram mesmo, ficou show de bola 👍👍</t>
+  </si>
+  <si>
+    <t>@loki_inluv vou pular</t>
+  </si>
+  <si>
+    <t>@melhornao777 @loki_trem @bakzinfx7 @loud_thurzin888 @bakzera quer falar de escrita mas o cara solta uma de "cabaço" kkkkkkkklkk</t>
+  </si>
+  <si>
+    <t>@wonderwidow meu deus o loki vai ficar até quando na marvel então</t>
+  </si>
+  <si>
+    <t>@umbrwa amg como que faz pra ser 100% loki me conta kkkk</t>
+  </si>
+  <si>
+    <t>meu deus
+escutando o peweecast do loki, e o marcelo é um ser insuportável pqp</t>
+  </si>
+  <si>
+    <t>o loki quando tiver um filho vai ser assim https://t.co/kds88dynug</t>
+  </si>
+  <si>
+    <t>@geovana_rodria nesse perfil proclamamos a religião de loki</t>
+  </si>
+  <si>
+    <t>@sithferrari 59 em não sei quantos anos quando o loki matou 80 em 2 dias, sim vdd</t>
+  </si>
+  <si>
+    <t>@leotswk tipo o povo falando do loki praticando incesto com si mesmo lkk</t>
+  </si>
+  <si>
+    <t>@iaemuriloo @morenothebest2 two novi traiu nathi com moreno</t>
+  </si>
+  <si>
+    <t>@fiorabairds @s0l4ngelo vei thor e loki quase mesma porcentagem</t>
+  </si>
+  <si>
+    <t>@i4virgil eu te amo tá bom, vc purê ellen eu loki e chloe pra sempre</t>
+  </si>
+  <si>
+    <t>@bylovelyy tudo sim, e com vc?</t>
+  </si>
+  <si>
+    <t>@vanoelove como a jeanne é tem a maldição acho impossível ela sobreviver pq de todos que vivos nenhum agora sobreviveu e me lembro do irmão do luca, o loki talvez se não matar a tempo ela fique que nem ele será? apesar de que o irmão até que tá controlável</t>
+  </si>
+  <si>
+    <t>✨thor: ragnarok✨
+9/10
+como é q pode um homem ser tão gostoso?
+amo o loki e ele juntos, tudo para todos
+adorei q odin morreu e q apareceu a primogênita
+achei meio viajado thor e hulk em outro planeta, apesar de bastante engraçado.
+a nova asgard promete, quero continuação</t>
+  </si>
+  <si>
+    <t>oi, me dá oi?</t>
+  </si>
+  <si>
+    <t>@pombodopru @peterjordan100 mas se um é consequencia do outro ñ faz sentido o loki pegar o bagulho tornar ele uma variante, sem esse fator os vingadores só iam pegar a jóia ali e voltar pro seu tempo</t>
+  </si>
+  <si>
+    <t>meu deus do nada bateu uma saudade do loki e da sylvie q dor</t>
+  </si>
+  <si>
+    <t>achava o loki feio, mas nessa série dele ai papai</t>
+  </si>
+  <si>
+    <t>@jojogum13 infelizmente não tenho tô trist</t>
+  </si>
+  <si>
+    <t>@fc_jjordan @bieltrk_ @loki_trem @pain_krzn @cacauzinha_ff @fluxo_alemaze tamo falando da merma org alex, rajah fluxo/ yuuri los grandes= nada haver mano, ale maze e two = fluxo, não pode é merma org 😁</t>
+  </si>
+  <si>
+    <t>@cohenw0rld sim mas é que pensando no gal tentando apunhalar o kian me lembrou da cena do loki kskskkkkk</t>
+  </si>
+  <si>
+    <t>@caatvante quem??</t>
+  </si>
+  <si>
+    <t>@duucarrasco qual foi loki</t>
+  </si>
+  <si>
+    <t>@cacaraujo2002 diga a verdade, você é o verdadeiro loki né? tem até o temp-pad, como pode ser tão rápida 0-0
+tá saltando no tempo</t>
+  </si>
+  <si>
+    <t>exatamente assim com messi e loki https://t.co/kwiq6i49ad</t>
+  </si>
+  <si>
+    <t>@pennysanroo @minottogustavo_ @tyedixie @feiticeiraescbr @marvelstudios multiverso ainda será + explorado: td caminha pra billy e tommy voltarem. o ucm deve juntar os jovens vingadores, eles devem ser a bola da vez. elizabeth olsen n renovou contrato ainda (q eu saiba) wandavision ainda n foi renovada! loki já. só ligar os pontos, pode acontecer...</t>
+  </si>
+  <si>
+    <t>o mobius esquecendo do loki💔💔💔💔💔💔💔💔</t>
+  </si>
+  <si>
+    <t>@joycelunass acho que o jhonatan majors talvez possa ser indicado a melhor ator convidado tbm</t>
+  </si>
+  <si>
+    <t>@pandora_kuru parece ter cheiro daqueles pão caseiro recém feito sabe bem quentinho adoro</t>
+  </si>
+  <si>
+    <t>acordei pra colocar o loki pra fora e meu pai tá jantando???? as 4 da manhã?????????</t>
+  </si>
+  <si>
+    <t>@puddingarts @loki_cb eu fui pior viu kakakaak</t>
+  </si>
+  <si>
+    <t>@bryanber5 a variante do loki, não irá comparecer pelo visto.</t>
+  </si>
+  <si>
+    <t>@inaba1guerreiro loki e suas variações...</t>
+  </si>
+  <si>
+    <t>qual seu top 5 da marvel?
+1- doutor estranho 
+2- feiticeira escarlate 
+3- capitã marvel 
+4- viuva negra 
+5- loki</t>
+  </si>
+  <si>
+    <t>https://t.co/gf7qq2lm8v
+📚 vote loki
+ ̷r̷$̷ ̷4̷9̷,̷9̷0̷
+r$ 39,90
+loki é muitas coisas: deus, trapaceiro, irmão, filho, vilão e até herói. agora, ele que adicionar mais uma coisa à lista: presidente dos estados unidos! é isso mesmo, o deus da trapaça quer ser o governante do ...</t>
+  </si>
+  <si>
+    <t>ai eu mudei de header pra essa de b99 que eu que fiz tambem 🤘
+o machadinho da gincana de rq
+saudades da loki era
+e essa bio horrorosa parece um trava zap 
+acho que eu tava meio depre na epoca ne 
+os firstprince na loc 😭😭😭😭 https://t.co/3xvfqxuqvd</t>
+  </si>
+  <si>
+    <t>@loki_inluv que amorzinho! &amp;lt;3</t>
+  </si>
+  <si>
+    <t>@hcneyhyvck não tô muito bem tbm mas tô levando</t>
+  </si>
+  <si>
+    <t>loki é mt foda</t>
+  </si>
+  <si>
+    <t>crl acordei quebrada e com o loki me perturbando ainda por cima q ódio</t>
+  </si>
+  <si>
+    <t>@loud_sofredor @loud_jordanxp azideia n vai morrer não loki akalala</t>
+  </si>
+  <si>
+    <t>@andremenino01 @loki_trem difícil yt buga com live assim</t>
+  </si>
+  <si>
+    <t>loki pq tao lindo</t>
+  </si>
+  <si>
+    <t>@melhornao777 @loki_trem @bakzinfx7 @loud_thurzin888 @bakzera o bom é saber que a noise com semanas apenas de montada ganharam o primeiro camp que jogaram, e foi nfa ta???? e sem contar que não pegaram os melhores jogadores da atualidade. já vcs pega os melhores achando que vão ganhar tudo kkk</t>
+  </si>
+  <si>
+    <t>toma no seu cu seu loki do caralho ta chapando jao ta achando oq meu truta</t>
+  </si>
+  <si>
+    <t>@clintarqueiro @bracinhodeferro @meupai_eadory amor pq ? @loki_l4ufeys0n</t>
+  </si>
+  <si>
+    <t>eu fico toda coisada pelo loki</t>
+  </si>
+  <si>
+    <t>@sylvielaufeydit @bracinhodeferro @meupai_eadory @loki_l4ufeys0n já sei ate oq ele vai falar</t>
+  </si>
+  <si>
+    <t>@kookvlong pode</t>
+  </si>
+  <si>
+    <t>amo a epifania q estou tendo com loki pq acho que já senti tudo isso q ele sente vendo esse absurdo em brisas distintas
+e sinceramente ele fala absurdo sempre q eu penso isso eh absurdo 
+perfeito</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2693,6 +3361,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2730,10 +3406,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2747,8 +3424,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3061,10 +3740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFC452E-675E-4E26-BABE-A1CA2946AE8C}">
-  <dimension ref="A1:B600"/>
+  <dimension ref="A1:B799"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A719" workbookViewId="0">
+      <selection activeCell="A601" sqref="A601:B799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7873,10 +8552,1602 @@
         <v>0</v>
       </c>
     </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A601" t="s">
+        <v>803</v>
+      </c>
+      <c r="B601">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A602" t="s">
+        <v>804</v>
+      </c>
+      <c r="B602">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A603" t="s">
+        <v>805</v>
+      </c>
+      <c r="B603">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A604" t="s">
+        <v>806</v>
+      </c>
+      <c r="B604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A605" t="s">
+        <v>807</v>
+      </c>
+      <c r="B605">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A606" t="s">
+        <v>808</v>
+      </c>
+      <c r="B606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A607" t="s">
+        <v>809</v>
+      </c>
+      <c r="B607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A608" t="s">
+        <v>810</v>
+      </c>
+      <c r="B608">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A609" t="s">
+        <v>811</v>
+      </c>
+      <c r="B609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A610" t="s">
+        <v>812</v>
+      </c>
+      <c r="B610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A611" t="s">
+        <v>813</v>
+      </c>
+      <c r="B611">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A612" t="s">
+        <v>814</v>
+      </c>
+      <c r="B612">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A613" t="s">
+        <v>815</v>
+      </c>
+      <c r="B613">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A614" t="s">
+        <v>816</v>
+      </c>
+      <c r="B614">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A615" t="s">
+        <v>817</v>
+      </c>
+      <c r="B615">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A616" t="s">
+        <v>818</v>
+      </c>
+      <c r="B616">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A617" t="s">
+        <v>819</v>
+      </c>
+      <c r="B617">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A618" t="s">
+        <v>820</v>
+      </c>
+      <c r="B618">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A619" t="s">
+        <v>821</v>
+      </c>
+      <c r="B619">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A620" t="s">
+        <v>822</v>
+      </c>
+      <c r="B620">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A621" t="s">
+        <v>823</v>
+      </c>
+      <c r="B621">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A622" t="s">
+        <v>824</v>
+      </c>
+      <c r="B622">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A623" t="s">
+        <v>825</v>
+      </c>
+      <c r="B623">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A624" t="s">
+        <v>826</v>
+      </c>
+      <c r="B624">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A625" t="s">
+        <v>827</v>
+      </c>
+      <c r="B625">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A626" t="s">
+        <v>828</v>
+      </c>
+      <c r="B626">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A627" t="s">
+        <v>829</v>
+      </c>
+      <c r="B627">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A628" t="s">
+        <v>830</v>
+      </c>
+      <c r="B628">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A629" t="s">
+        <v>831</v>
+      </c>
+      <c r="B629">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A630" t="s">
+        <v>832</v>
+      </c>
+      <c r="B630">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A631" t="s">
+        <v>833</v>
+      </c>
+      <c r="B631">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A632" t="s">
+        <v>834</v>
+      </c>
+      <c r="B632">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A633" t="s">
+        <v>835</v>
+      </c>
+      <c r="B633">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A634" t="s">
+        <v>836</v>
+      </c>
+      <c r="B634">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A635" t="s">
+        <v>837</v>
+      </c>
+      <c r="B635">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A636" t="s">
+        <v>838</v>
+      </c>
+      <c r="B636">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A637" t="s">
+        <v>839</v>
+      </c>
+      <c r="B637">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A638" t="s">
+        <v>840</v>
+      </c>
+      <c r="B638">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A639" t="s">
+        <v>841</v>
+      </c>
+      <c r="B639">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A640" t="s">
+        <v>842</v>
+      </c>
+      <c r="B640">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A641" t="s">
+        <v>843</v>
+      </c>
+      <c r="B641">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A642" t="s">
+        <v>844</v>
+      </c>
+      <c r="B642">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A643" t="s">
+        <v>845</v>
+      </c>
+      <c r="B643">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A644" t="s">
+        <v>846</v>
+      </c>
+      <c r="B644">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A645" t="s">
+        <v>847</v>
+      </c>
+      <c r="B645">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A646" t="s">
+        <v>848</v>
+      </c>
+      <c r="B646">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A647" t="s">
+        <v>849</v>
+      </c>
+      <c r="B647">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A648" t="s">
+        <v>850</v>
+      </c>
+      <c r="B648">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A649" t="s">
+        <v>851</v>
+      </c>
+      <c r="B649">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A650" t="s">
+        <v>852</v>
+      </c>
+      <c r="B650">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A651" t="s">
+        <v>853</v>
+      </c>
+      <c r="B651">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A652" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A653" t="s">
+        <v>855</v>
+      </c>
+      <c r="B653">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A654" t="s">
+        <v>856</v>
+      </c>
+      <c r="B654">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A655" t="s">
+        <v>857</v>
+      </c>
+      <c r="B655">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A656" t="s">
+        <v>858</v>
+      </c>
+      <c r="B656">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A657" t="s">
+        <v>859</v>
+      </c>
+      <c r="B657">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A658" t="s">
+        <v>860</v>
+      </c>
+      <c r="B658">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A659" t="s">
+        <v>861</v>
+      </c>
+      <c r="B659">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A660" t="s">
+        <v>862</v>
+      </c>
+      <c r="B660">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A661" t="s">
+        <v>863</v>
+      </c>
+      <c r="B661">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A662" t="s">
+        <v>864</v>
+      </c>
+      <c r="B662">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A663" t="s">
+        <v>865</v>
+      </c>
+      <c r="B663">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A664" t="s">
+        <v>866</v>
+      </c>
+      <c r="B664">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A665" t="s">
+        <v>867</v>
+      </c>
+      <c r="B665">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A666" t="s">
+        <v>868</v>
+      </c>
+      <c r="B666">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A667" t="s">
+        <v>869</v>
+      </c>
+      <c r="B667">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A668" t="s">
+        <v>870</v>
+      </c>
+      <c r="B668">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A669" t="s">
+        <v>871</v>
+      </c>
+      <c r="B669">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A670" t="s">
+        <v>872</v>
+      </c>
+      <c r="B670">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A671" t="s">
+        <v>873</v>
+      </c>
+      <c r="B671">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A672" t="s">
+        <v>874</v>
+      </c>
+      <c r="B672">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A673" t="s">
+        <v>875</v>
+      </c>
+      <c r="B673">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A674" t="s">
+        <v>876</v>
+      </c>
+      <c r="B674">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A675" t="s">
+        <v>877</v>
+      </c>
+      <c r="B675">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A676" t="s">
+        <v>878</v>
+      </c>
+      <c r="B676">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A677" t="s">
+        <v>879</v>
+      </c>
+      <c r="B677">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A678" t="s">
+        <v>880</v>
+      </c>
+      <c r="B678">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A679" t="s">
+        <v>881</v>
+      </c>
+      <c r="B679">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A680" t="s">
+        <v>882</v>
+      </c>
+      <c r="B680">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A681" t="s">
+        <v>883</v>
+      </c>
+      <c r="B681">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A682" t="s">
+        <v>884</v>
+      </c>
+      <c r="B682">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A683" t="s">
+        <v>885</v>
+      </c>
+      <c r="B683">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A684" t="s">
+        <v>886</v>
+      </c>
+      <c r="B684">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A685" t="s">
+        <v>887</v>
+      </c>
+      <c r="B685">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A686" t="s">
+        <v>888</v>
+      </c>
+      <c r="B686">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A687" t="s">
+        <v>889</v>
+      </c>
+      <c r="B687">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A688" t="s">
+        <v>890</v>
+      </c>
+      <c r="B688">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A689" t="s">
+        <v>891</v>
+      </c>
+      <c r="B689">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A690" t="s">
+        <v>892</v>
+      </c>
+      <c r="B690">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A691" t="s">
+        <v>893</v>
+      </c>
+      <c r="B691">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A692" t="s">
+        <v>894</v>
+      </c>
+      <c r="B692">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A693" t="s">
+        <v>895</v>
+      </c>
+      <c r="B693">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A694" t="s">
+        <v>896</v>
+      </c>
+      <c r="B694">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A695" t="s">
+        <v>897</v>
+      </c>
+      <c r="B695">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A696" t="s">
+        <v>898</v>
+      </c>
+      <c r="B696">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A697" t="s">
+        <v>899</v>
+      </c>
+      <c r="B697">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A698" t="s">
+        <v>900</v>
+      </c>
+      <c r="B698">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A699" t="s">
+        <v>901</v>
+      </c>
+      <c r="B699">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A700" t="s">
+        <v>902</v>
+      </c>
+      <c r="B700">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A701" t="s">
+        <v>903</v>
+      </c>
+      <c r="B701">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A702" t="s">
+        <v>904</v>
+      </c>
+      <c r="B702">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A703" t="s">
+        <v>905</v>
+      </c>
+      <c r="B703">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A704" t="s">
+        <v>906</v>
+      </c>
+      <c r="B704">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A705" t="s">
+        <v>907</v>
+      </c>
+      <c r="B705">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A706" t="s">
+        <v>908</v>
+      </c>
+      <c r="B706">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A707" t="s">
+        <v>909</v>
+      </c>
+      <c r="B707">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A708" t="s">
+        <v>910</v>
+      </c>
+      <c r="B708">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A709" t="s">
+        <v>911</v>
+      </c>
+      <c r="B709">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A710" t="s">
+        <v>912</v>
+      </c>
+      <c r="B710">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A711" t="s">
+        <v>913</v>
+      </c>
+      <c r="B711">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A712" t="s">
+        <v>914</v>
+      </c>
+      <c r="B712">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A713" t="s">
+        <v>915</v>
+      </c>
+      <c r="B713">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A714" t="s">
+        <v>916</v>
+      </c>
+      <c r="B714">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A715" t="s">
+        <v>917</v>
+      </c>
+      <c r="B715">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A716" t="s">
+        <v>918</v>
+      </c>
+      <c r="B716">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A717" t="s">
+        <v>919</v>
+      </c>
+      <c r="B717">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A718" t="s">
+        <v>920</v>
+      </c>
+      <c r="B718">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A719" t="s">
+        <v>921</v>
+      </c>
+      <c r="B719">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A720" t="s">
+        <v>922</v>
+      </c>
+      <c r="B720">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A721" t="s">
+        <v>923</v>
+      </c>
+      <c r="B721">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A722" t="s">
+        <v>924</v>
+      </c>
+      <c r="B722">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+      <c r="A723" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="B723">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A724" t="s">
+        <v>926</v>
+      </c>
+      <c r="B724">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A725" t="s">
+        <v>927</v>
+      </c>
+      <c r="B725">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A726" t="s">
+        <v>928</v>
+      </c>
+      <c r="B726">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A727" t="s">
+        <v>929</v>
+      </c>
+      <c r="B727">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A728" t="s">
+        <v>930</v>
+      </c>
+      <c r="B728">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A729" t="s">
+        <v>931</v>
+      </c>
+      <c r="B729">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A730" t="s">
+        <v>932</v>
+      </c>
+      <c r="B730">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A731" t="s">
+        <v>933</v>
+      </c>
+      <c r="B731">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A732" t="s">
+        <v>934</v>
+      </c>
+      <c r="B732">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A733" t="s">
+        <v>935</v>
+      </c>
+      <c r="B733">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A734" t="s">
+        <v>936</v>
+      </c>
+      <c r="B734">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A735" t="s">
+        <v>937</v>
+      </c>
+      <c r="B735">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A736" t="s">
+        <v>938</v>
+      </c>
+      <c r="B736">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A737" t="s">
+        <v>939</v>
+      </c>
+      <c r="B737">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A738" t="s">
+        <v>940</v>
+      </c>
+      <c r="B738">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A739" t="s">
+        <v>941</v>
+      </c>
+      <c r="B739">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A740" t="s">
+        <v>942</v>
+      </c>
+      <c r="B740">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A741" t="s">
+        <v>943</v>
+      </c>
+      <c r="B741">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A742" t="s">
+        <v>944</v>
+      </c>
+      <c r="B742">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A743" t="s">
+        <v>945</v>
+      </c>
+      <c r="B743">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A744" t="s">
+        <v>946</v>
+      </c>
+      <c r="B744">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A745" t="s">
+        <v>947</v>
+      </c>
+      <c r="B745">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A746" t="s">
+        <v>948</v>
+      </c>
+      <c r="B746">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A747" t="s">
+        <v>949</v>
+      </c>
+      <c r="B747">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A748" t="s">
+        <v>950</v>
+      </c>
+      <c r="B748">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A749" t="s">
+        <v>951</v>
+      </c>
+      <c r="B749">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A750" t="s">
+        <v>952</v>
+      </c>
+      <c r="B750">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A751" t="s">
+        <v>953</v>
+      </c>
+      <c r="B751">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A752" t="s">
+        <v>954</v>
+      </c>
+      <c r="B752">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A753" t="s">
+        <v>955</v>
+      </c>
+      <c r="B753">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A754" t="s">
+        <v>956</v>
+      </c>
+      <c r="B754">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A755" t="s">
+        <v>957</v>
+      </c>
+      <c r="B755">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A756" t="s">
+        <v>958</v>
+      </c>
+      <c r="B756">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A757" t="s">
+        <v>959</v>
+      </c>
+      <c r="B757">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A758" t="s">
+        <v>960</v>
+      </c>
+      <c r="B758">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A759" t="s">
+        <v>961</v>
+      </c>
+      <c r="B759">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A760" t="s">
+        <v>962</v>
+      </c>
+      <c r="B760">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A761" t="s">
+        <v>963</v>
+      </c>
+      <c r="B761">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A762" t="s">
+        <v>964</v>
+      </c>
+      <c r="B762">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="763" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A763" t="s">
+        <v>965</v>
+      </c>
+      <c r="B763">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A764" t="s">
+        <v>966</v>
+      </c>
+      <c r="B764">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A765" t="s">
+        <v>967</v>
+      </c>
+      <c r="B765">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A766" t="s">
+        <v>968</v>
+      </c>
+      <c r="B766">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A767" t="s">
+        <v>969</v>
+      </c>
+      <c r="B767">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A768" t="s">
+        <v>970</v>
+      </c>
+      <c r="B768">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A769" t="s">
+        <v>971</v>
+      </c>
+      <c r="B769">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A770" t="s">
+        <v>972</v>
+      </c>
+      <c r="B770">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A771" t="s">
+        <v>973</v>
+      </c>
+      <c r="B771">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A772" t="s">
+        <v>974</v>
+      </c>
+      <c r="B772">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A773" t="s">
+        <v>975</v>
+      </c>
+      <c r="B773">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A774" t="s">
+        <v>976</v>
+      </c>
+      <c r="B774">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A775" t="s">
+        <v>977</v>
+      </c>
+      <c r="B775">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A776" t="s">
+        <v>978</v>
+      </c>
+      <c r="B776">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A777" t="s">
+        <v>979</v>
+      </c>
+      <c r="B777">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A778" t="s">
+        <v>980</v>
+      </c>
+      <c r="B778">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A779" t="s">
+        <v>981</v>
+      </c>
+      <c r="B779">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A780" t="s">
+        <v>982</v>
+      </c>
+      <c r="B780">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A781" t="s">
+        <v>983</v>
+      </c>
+      <c r="B781">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A782" t="s">
+        <v>984</v>
+      </c>
+      <c r="B782">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A783" t="s">
+        <v>985</v>
+      </c>
+      <c r="B783">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="784" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A784" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="B784">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A785" t="s">
+        <v>987</v>
+      </c>
+      <c r="B785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A786" t="s">
+        <v>988</v>
+      </c>
+      <c r="B786">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A787" t="s">
+        <v>989</v>
+      </c>
+      <c r="B787">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A788" t="s">
+        <v>990</v>
+      </c>
+      <c r="B788">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="789" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A789" t="s">
+        <v>991</v>
+      </c>
+      <c r="B789">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A790" t="s">
+        <v>992</v>
+      </c>
+      <c r="B790">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A791" t="s">
+        <v>993</v>
+      </c>
+      <c r="B791">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A792" t="s">
+        <v>994</v>
+      </c>
+      <c r="B792">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A793" t="s">
+        <v>995</v>
+      </c>
+      <c r="B793">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A794" t="s">
+        <v>996</v>
+      </c>
+      <c r="B794">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A795" t="s">
+        <v>997</v>
+      </c>
+      <c r="B795">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="796" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A796" t="s">
+        <v>998</v>
+      </c>
+      <c r="B796">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A797" t="s">
+        <v>999</v>
+      </c>
+      <c r="B797">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A798" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B798">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A799" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B799">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B801" xr:uid="{4DFC452E-675E-4E26-BABE-A1CA2946AE8C}"/>
+  <hyperlinks>
+    <hyperlink ref="A784" r:id="rId1" xr:uid="{5CE7EBCE-E1BF-4BD4-BE97-2615D2FAF65D}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7884,7 +10155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F687F0-AA3C-4394-BCF6-5AA3B57C7D46}">
   <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A78" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7902,7 +10173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>420</v>
       </c>
@@ -7910,7 +10181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>432</v>
       </c>
@@ -7950,7 +10221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>293</v>
       </c>
@@ -7974,7 +10245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>72</v>
       </c>
@@ -7982,7 +10253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>280</v>
       </c>
@@ -7990,7 +10261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
@@ -8006,7 +10277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>77</v>
       </c>
@@ -8022,7 +10293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>227</v>
       </c>
@@ -8038,7 +10309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>533</v>
       </c>
@@ -8046,7 +10317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>63</v>
       </c>
@@ -8070,7 +10341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>435</v>
       </c>
@@ -8078,7 +10349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>496</v>
       </c>
@@ -8086,7 +10357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -8094,7 +10365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>118</v>
       </c>
@@ -8102,7 +10373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>443</v>
       </c>
@@ -8174,7 +10445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>127</v>
       </c>
@@ -8190,7 +10461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>332</v>
       </c>
@@ -8214,7 +10485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>261</v>
       </c>
@@ -8230,7 +10501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>506</v>
       </c>
@@ -8270,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>472</v>
       </c>
@@ -8286,7 +10557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="261" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>219</v>
       </c>
@@ -8302,7 +10573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>301</v>
       </c>
@@ -8310,7 +10581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>516</v>
       </c>
@@ -8318,7 +10589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>311</v>
       </c>
@@ -8334,7 +10605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>74</v>
       </c>
@@ -8342,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>147</v>
       </c>
@@ -8350,7 +10621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>473</v>
       </c>
@@ -8358,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>569</v>
       </c>
@@ -8366,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>115</v>
       </c>
@@ -8382,7 +10653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>470</v>
       </c>
@@ -8390,7 +10661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>411</v>
       </c>
@@ -8422,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>599</v>
       </c>
@@ -8446,7 +10717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>224</v>
       </c>
@@ -8462,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>133</v>
       </c>
@@ -8494,7 +10765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>186</v>
       </c>
@@ -8502,7 +10773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>572</v>
       </c>
@@ -8526,7 +10797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>179</v>
       </c>
@@ -8534,7 +10805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="319" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>307</v>
       </c>
@@ -8542,7 +10813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>354</v>
       </c>
@@ -8558,7 +10829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>211</v>
       </c>
@@ -8574,7 +10845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>141</v>
       </c>
@@ -8582,7 +10853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>551</v>
       </c>
@@ -8590,7 +10861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>513</v>
       </c>
@@ -8598,7 +10869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>489</v>
       </c>
@@ -8606,7 +10877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>144</v>
       </c>
@@ -8614,7 +10885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>66</v>
       </c>
@@ -8622,7 +10893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="319" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>532</v>
       </c>
@@ -8630,7 +10901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>62</v>
       </c>
@@ -8646,7 +10917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>151</v>
       </c>
@@ -8662,7 +10933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>175</v>
       </c>
@@ -8670,7 +10941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>529</v>
       </c>
@@ -8686,7 +10957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>232</v>
       </c>
@@ -8694,7 +10965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>377</v>
       </c>
@@ -8702,7 +10973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>423</v>
       </c>
@@ -8718,7 +10989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>503</v>
       </c>
@@ -8726,7 +10997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>543</v>
       </c>
@@ -8734,7 +11005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>199</v>
       </c>
@@ -8750,7 +11021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>236</v>
       </c>
@@ -8758,7 +11029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>557</v>
       </c>
@@ -8766,7 +11037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>337</v>
       </c>
@@ -8774,7 +11045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>155</v>
       </c>
@@ -8798,7 +11069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>361</v>
       </c>
@@ -8806,7 +11077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>436</v>
       </c>
@@ -8814,7 +11085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>462</v>
       </c>
@@ -8830,7 +11101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>137</v>
       </c>
@@ -8838,7 +11109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>309</v>
       </c>
@@ -8846,7 +11117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>106</v>
       </c>
@@ -8854,7 +11125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>109</v>
       </c>
@@ -8862,7 +11133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>341</v>
       </c>
@@ -8878,7 +11149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>406</v>
       </c>
@@ -8886,7 +11157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>20</v>
       </c>
@@ -8894,7 +11165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>213</v>
       </c>
@@ -8910,7 +11181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>229</v>
       </c>
@@ -8918,7 +11189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>369</v>
       </c>
@@ -8934,7 +11205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>509</v>
       </c>
@@ -8942,7 +11213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>484</v>
       </c>
@@ -8950,7 +11221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>93</v>
       </c>
@@ -8958,7 +11229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>203</v>
       </c>
@@ -8966,7 +11237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>370</v>
       </c>
@@ -8974,7 +11245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>200</v>
       </c>
@@ -8982,7 +11253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>97</v>
       </c>
@@ -8990,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>69</v>
       </c>
@@ -8998,7 +11269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>459</v>
       </c>
@@ -9006,7 +11277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>269</v>
       </c>
@@ -9014,7 +11285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>78</v>
       </c>
@@ -9022,7 +11293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>177</v>
       </c>
@@ -9030,7 +11301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>365</v>
       </c>
@@ -9038,7 +11309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>391</v>
       </c>
@@ -9054,7 +11325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>398</v>
       </c>
@@ -9062,7 +11333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>431</v>
       </c>
@@ -9078,7 +11349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>23</v>
       </c>
@@ -9086,7 +11357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>497</v>
       </c>
@@ -9094,7 +11365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
         <v>257</v>
       </c>
@@ -9102,7 +11373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>149</v>
       </c>
@@ -9110,7 +11381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
         <v>338</v>
       </c>
@@ -9126,7 +11397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="s">
         <v>90</v>
       </c>
@@ -9158,7 +11429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
         <v>457</v>
       </c>
@@ -9166,7 +11437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="s">
         <v>486</v>
       </c>
@@ -9174,7 +11445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="s">
         <v>55</v>
       </c>
@@ -9182,7 +11453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
         <v>424</v>
       </c>
@@ -9190,7 +11461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="s">
         <v>51</v>
       </c>
@@ -9206,7 +11477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="261" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
         <v>368</v>
       </c>
@@ -9214,7 +11485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
         <v>217</v>
       </c>
@@ -9222,7 +11493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="s">
         <v>366</v>
       </c>
@@ -9230,7 +11501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
         <v>325</v>
       </c>
@@ -9238,7 +11509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A169" s="3" t="s">
         <v>187</v>
       </c>
@@ -9246,7 +11517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="s">
         <v>476</v>
       </c>
@@ -9254,7 +11525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="s">
         <v>433</v>
       </c>
@@ -9270,7 +11541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="s">
         <v>270</v>
       </c>
@@ -9278,7 +11549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
         <v>283</v>
       </c>
@@ -9286,7 +11557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="s">
         <v>344</v>
       </c>
@@ -9294,7 +11565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
         <v>204</v>
       </c>
@@ -9302,7 +11573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="s">
         <v>468</v>
       </c>
@@ -9310,7 +11581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
         <v>259</v>
       </c>
@@ -9318,7 +11589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
         <v>417</v>
       </c>
@@ -9326,7 +11597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="s">
         <v>596</v>
       </c>
@@ -9334,7 +11605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A181" s="3" t="s">
         <v>504</v>
       </c>
@@ -9342,7 +11613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="s">
         <v>61</v>
       </c>
@@ -9350,7 +11621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
         <v>277</v>
       </c>
@@ -9358,7 +11629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
         <v>158</v>
       </c>
@@ -9366,7 +11637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="s">
         <v>518</v>
       </c>
@@ -9374,7 +11645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
         <v>502</v>
       </c>
@@ -9382,7 +11653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="s">
         <v>191</v>
       </c>
@@ -9398,7 +11669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="s">
         <v>174</v>
       </c>
@@ -9406,7 +11677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
         <v>131</v>
       </c>
@@ -9414,7 +11685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="319" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A191" s="3" t="s">
         <v>190</v>
       </c>
@@ -9422,7 +11693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A192" s="3" t="s">
         <v>565</v>
       </c>
@@ -9430,7 +11701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="3" t="s">
         <v>304</v>
       </c>
@@ -9438,7 +11709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A194" s="3" t="s">
         <v>243</v>
       </c>
@@ -9454,7 +11725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="3" t="s">
         <v>254</v>
       </c>
@@ -9462,7 +11733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="3" t="s">
         <v>510</v>
       </c>
@@ -9470,7 +11741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A198" s="3" t="s">
         <v>207</v>
       </c>
@@ -9478,7 +11749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A199" s="3" t="s">
         <v>263</v>
       </c>
@@ -9486,7 +11757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="3" t="s">
         <v>409</v>
       </c>
@@ -9502,7 +11773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="3" t="s">
         <v>215</v>
       </c>

</xml_diff>